<commit_message>
fixed some errors in documentation
</commit_message>
<xml_diff>
--- a/resourses/Project 1 Arduino ini.xlsx
+++ b/resourses/Project 1 Arduino ini.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanew\Desktop\Boiler_Control\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dany\Desktop\Boiler_Control\resourses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Serial</t>
   </si>
@@ -237,9 +237,6 @@
   </si>
   <si>
     <t>BTempSet</t>
-  </si>
-  <si>
-    <t>BTemp</t>
   </si>
   <si>
     <t>BHistSet</t>
@@ -345,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,6 +359,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,61 +654,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G43"/>
+  <dimension ref="B3:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="5" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="5" width="15.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -718,14 +718,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
@@ -733,14 +733,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
@@ -748,14 +748,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
@@ -763,24 +763,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -793,14 +793,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="2" t="s">
         <v>32</v>
       </c>
@@ -811,14 +811,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
@@ -829,14 +829,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="2" t="s">
         <v>36</v>
       </c>
@@ -847,14 +847,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="2" t="s">
         <v>38</v>
       </c>
@@ -865,14 +865,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
@@ -883,14 +883,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="2" t="s">
         <v>42</v>
       </c>
@@ -901,14 +901,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
@@ -919,14 +919,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -939,14 +939,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="3" t="s">
         <v>62</v>
       </c>
@@ -957,41 +957,41 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C30" s="10" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>0</v>
       </c>
@@ -1002,8 +1002,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
+        <f>C31 + E32</f>
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1013,8 +1014,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="1">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="10">
+        <f t="shared" ref="C33:C42" si="0">C32 + E33</f>
         <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1024,8 +1026,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="1">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="10">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1035,8 +1038,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35" s="1">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="10">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1046,19 +1050,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="1">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="10">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C37" s="1">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="10">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1068,8 +1074,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C38" s="1">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1079,8 +1086,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C39" s="1">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="10">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1090,50 +1098,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C40" s="1">
-        <v>10</v>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="10">
+        <f>32</f>
+        <v>32</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C41" s="1">
-        <f>C40+32</f>
-        <v>42</v>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="10">
+        <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E41" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="1">
-        <f>C41+32</f>
-        <v>74</v>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="10">
+        <f t="shared" si="0"/>
+        <v>106</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E42" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C43" s="1">
-        <f>C42+32</f>
-        <v>106</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="1">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated excel file and changed update algorithm
</commit_message>
<xml_diff>
--- a/resourses/Project 1 Arduino ini.xlsx
+++ b/resourses/Project 1 Arduino ini.xlsx
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>Serial</t>
   </si>
   <si>
-    <t>TX0</t>
-  </si>
-  <si>
-    <t>RX0</t>
-  </si>
-  <si>
     <t>NEXTION</t>
   </si>
   <si>
@@ -44,12 +38,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>DS18B20</t>
   </si>
   <si>
@@ -59,63 +47,18 @@
     <t>Температура подово</t>
   </si>
   <si>
-    <t>Температура колектор</t>
-  </si>
-  <si>
     <t>Комуникация</t>
   </si>
   <si>
     <t>Outputs</t>
   </si>
   <si>
-    <t>D31</t>
-  </si>
-  <si>
-    <t>D33</t>
-  </si>
-  <si>
-    <t>D35</t>
-  </si>
-  <si>
-    <t>D37</t>
-  </si>
-  <si>
-    <t>D39</t>
-  </si>
-  <si>
-    <t>D41</t>
-  </si>
-  <si>
-    <t>D43</t>
-  </si>
-  <si>
-    <t>D45</t>
-  </si>
-  <si>
-    <t>D47</t>
-  </si>
-  <si>
-    <t>D49</t>
-  </si>
-  <si>
-    <t>D51</t>
-  </si>
-  <si>
-    <t>D53</t>
-  </si>
-  <si>
-    <t>RELAY BLOCK        1-8</t>
-  </si>
-  <si>
     <t>DISPLAY</t>
   </si>
   <si>
     <t>TEMPERTURE SENSORS</t>
   </si>
   <si>
-    <t>RELAY BLOCK        1-4</t>
-  </si>
-  <si>
     <t>RELAY 1</t>
   </si>
   <si>
@@ -206,9 +149,6 @@
     <t>RemoteHeater</t>
   </si>
   <si>
-    <t>Температура стайна</t>
-  </si>
-  <si>
     <t>RELAY 9</t>
   </si>
   <si>
@@ -246,13 +186,82 @@
   </si>
   <si>
     <t>BoilerPic</t>
+  </si>
+  <si>
+    <t>Variable size in bytes</t>
+  </si>
+  <si>
+    <t>RELAY BLOCK        8-1</t>
+  </si>
+  <si>
+    <t>RELAY BLOCK        4-1</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>D34</t>
+  </si>
+  <si>
+    <t>D36</t>
+  </si>
+  <si>
+    <t>D38</t>
+  </si>
+  <si>
+    <t>D40</t>
+  </si>
+  <si>
+    <t>D42</t>
+  </si>
+  <si>
+    <t>D44</t>
+  </si>
+  <si>
+    <t>D46</t>
+  </si>
+  <si>
+    <t>D48</t>
+  </si>
+  <si>
+    <t>D52</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>TX1</t>
+  </si>
+  <si>
+    <t>RX1</t>
+  </si>
+  <si>
+    <t>RELAY BLOCK     4-1</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>D24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +278,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -338,11 +354,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,8 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,11 +394,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,17 +688,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G42"/>
+  <dimension ref="B3:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
@@ -676,46 +711,46 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>12</v>
+      <c r="F4" s="13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+        <v>70</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -723,425 +758,446 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="11"/>
       <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
-        <v>55</v>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
       <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>26</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D16" s="11"/>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="12"/>
+        <v>60</v>
+      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
         <v>33</v>
-      </c>
-      <c r="G17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>61</v>
+      </c>
+      <c r="D18" s="11"/>
       <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
         <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="D19" s="11"/>
       <c r="E19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="D20" s="11"/>
       <c r="E20" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
         <v>39</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="D21" s="11"/>
       <c r="E21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
         <v>40</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>43</v>
+        <v>65</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D24" s="11"/>
       <c r="E24" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="D25" s="11"/>
       <c r="E25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="3" t="s">
-        <v>63</v>
+      <c r="B26" s="9">
+        <v>13</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
-        <v>12</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="B27" s="9">
+        <v>14</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="8"/>
+      <c r="B29" s="9">
+        <v>16</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
         <v>0</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
-        <f>C31 + E32</f>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <f>C34 + E35</f>
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="10">
-        <f t="shared" ref="C33:C42" si="0">C32 + E33</f>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="8">
+        <f t="shared" ref="C36:C45" si="0">C35 + E36</f>
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="D36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="10">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="10">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="1">
+      <c r="D38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="10">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="D39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="10">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="D40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="10">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="D41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E41" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="10">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="D42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="10">
-        <f>32</f>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="8">
         <v>32</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="D43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="10">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="8">
         <v>74</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="1">
+      <c r="D44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="10">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="8">
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="D45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="1">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="D24:D27"/>
+  <mergeCells count="9">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="D22:D25"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D16:D23"/>
+    <mergeCell ref="D14:D21"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E26:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>